<commit_message>
US-12530 [IMP] Import function + checks + update import template
</commit_message>
<xml_diff>
--- a/bin/addons/msf_accrual/wizard/Accrual_Lines_Import_Template_File.xlsx
+++ b/bin/addons/msf_accrual/wizard/Accrual_Lines_Import_Template_File.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22125" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18450" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Accrual Lines" sheetId="1" r:id="rId1"/>
@@ -19,20 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Account</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Unit Price</t>
-  </si>
-  <si>
     <t>Destination</t>
   </si>
   <si>
@@ -40,6 +31,54 @@
   </si>
   <si>
     <t>Funding Pool</t>
+  </si>
+  <si>
+    <t>OPS</t>
+  </si>
+  <si>
+    <t>MW101</t>
+  </si>
+  <si>
+    <t>PF</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Accrual Amount Booking</t>
+  </si>
+  <si>
+    <t>Expense Account</t>
+  </si>
+  <si>
+    <t>ref</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>desc2</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>desc3</t>
+  </si>
+  <si>
+    <t>ref3</t>
+  </si>
+  <si>
+    <t>20;35;45</t>
+  </si>
+  <si>
+    <t>MW101;MW100;MW110</t>
+  </si>
+  <si>
+    <t>OPS;OPS;OPS</t>
+  </si>
+  <si>
+    <t>PF;PF;PF</t>
   </si>
 </sst>
 </file>
@@ -418,39 +457,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="7" width="15" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="5" width="23.42578125" customWidth="1"/>
+    <col min="6" max="8" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>60000</v>
+      </c>
+      <c r="D2">
+        <v>150</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="H2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>60000</v>
+      </c>
+      <c r="D3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>60000</v>
+      </c>
+      <c r="D4">
+        <v>300</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
US-12530 [IMP] Preload the template file in the wizard in order to have the Save As button displayed + Removed not anymore used code for the old button to generate the import file template
</commit_message>
<xml_diff>
--- a/bin/addons/msf_accrual/wizard/Accrual_Lines_Import_Template_File.xlsx
+++ b/bin/addons/msf_accrual/wizard/Accrual_Lines_Import_Template_File.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18450" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22125" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Accrual Lines" sheetId="1" r:id="rId1"/>
@@ -19,66 +19,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Description</t>
   </si>
   <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Expense Account</t>
+  </si>
+  <si>
+    <t>Accrual Amount Booking</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Cost Center</t>
+  </si>
+  <si>
     <t>Destination</t>
   </si>
   <si>
-    <t>Cost Center</t>
-  </si>
-  <si>
     <t>Funding Pool</t>
-  </si>
-  <si>
-    <t>OPS</t>
-  </si>
-  <si>
-    <t>MW101</t>
-  </si>
-  <si>
-    <t>PF</t>
-  </si>
-  <si>
-    <t>Reference</t>
-  </si>
-  <si>
-    <t>Accrual Amount Booking</t>
-  </si>
-  <si>
-    <t>Expense Account</t>
-  </si>
-  <si>
-    <t>ref</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>desc2</t>
-  </si>
-  <si>
-    <t>Percentage</t>
-  </si>
-  <si>
-    <t>desc3</t>
-  </si>
-  <si>
-    <t>ref3</t>
-  </si>
-  <si>
-    <t>20;35;45</t>
-  </si>
-  <si>
-    <t>MW101;MW100;MW110</t>
-  </si>
-  <si>
-    <t>OPS;OPS;OPS</t>
-  </si>
-  <si>
-    <t>PF;PF;PF</t>
   </si>
 </sst>
 </file>
@@ -146,12 +110,16 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -457,108 +425,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="8" width="15" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
+    <col min="5" max="8" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>60000</v>
-      </c>
-      <c r="D2">
-        <v>150</v>
-      </c>
-      <c r="E2">
-        <v>100</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>60000</v>
-      </c>
-      <c r="D3">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4">
-        <v>60000</v>
-      </c>
-      <c r="D4">
-        <v>300</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>